<commit_message>
Added a window listener to catch the frame closing event, which will bring up a confirmation prompt before actually closing.
</commit_message>
<xml_diff>
--- a/Adventurer/Adv_UseCases/A00_InitQuit/INIT_TestSummary.xlsx
+++ b/Adventurer/Adv_UseCases/A00_InitQuit/INIT_TestSummary.xlsx
@@ -143,7 +143,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -232,6 +232,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -321,7 +328,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -379,6 +386,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="29">
@@ -784,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -845,75 +858,75 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:7" ht="36">
+    <row r="5" spans="1:7" ht="39">
       <c r="A5" s="10">
         <v>1</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="25" t="s">
         <v>30</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="24">
+    <row r="6" spans="1:7" ht="26">
       <c r="A6" s="3">
         <v>2</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="25" t="s">
         <v>32</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="24">
+    <row r="7" spans="1:7" ht="26">
       <c r="A7" s="3">
         <v>3</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="25" t="s">
         <v>32</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="24">
+    <row r="8" spans="1:7" ht="26">
       <c r="A8" s="3">
         <v>4</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="25" t="s">
         <v>35</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="24">
+    <row r="9" spans="1:7" ht="26">
       <c r="A9" s="3">
         <v>5</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="25" t="s">
         <v>37</v>
       </c>
       <c r="E9" s="2"/>

</xml_diff>